<commit_message>
Moved few resistors for proper alignment
</commit_message>
<xml_diff>
--- a/cam/RP2040-ProMini-20230613-CPL.xlsx
+++ b/cam/RP2040-ProMini-20230613-CPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-ProMini\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A54646-3773-4E08-B59B-C1C13FD73EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04A330D-0745-4773-978F-A04477A11506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23040" yWindow="0" windowWidth="23040" windowHeight="25320" xr2:uid="{1DC8C5A6-54F6-45D4-9EBD-5B030B60A142}"/>
+    <workbookView xWindow="216" yWindow="4164" windowWidth="26388" windowHeight="20412" xr2:uid="{1DC8C5A6-54F6-45D4-9EBD-5B030B60A142}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +869,7 @@
         <v>147.32</v>
       </c>
       <c r="C21">
-        <v>-102.36</v>
+        <v>-102.235</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -886,7 +886,7 @@
         <v>146.05000000000001</v>
       </c>
       <c r="C22">
-        <v>-102.36</v>
+        <v>-102.235</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>

</xml_diff>